<commit_message>
Ajustes imagenes tema 3 mat 6
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado06/guion03/SolicitudGrafica MA_06_03_CO.xlsx
+++ b/fuentes/contenidos/grado06/guion03/SolicitudGrafica MA_06_03_CO.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EDITORIAL PLANETA\TEMA 3\EDICION 2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DianaMargarita\Documents\GitHub\Matematicas\fuentes\contenidos\grado06\guion03\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="189">
   <si>
     <t>Fecha:</t>
   </si>
@@ -567,9 +567,6 @@
     <t>Boletería de una función de teatro</t>
   </si>
   <si>
-    <t>Quitar descripción.</t>
-  </si>
-  <si>
     <t>IMG07</t>
   </si>
   <si>
@@ -587,6 +584,63 @@
   <si>
     <t>Cambiar la palabra Resto por Residuo. 
 Es necesario cambiar el punto del número 1054</t>
+  </si>
+  <si>
+    <t>IMG19</t>
+  </si>
+  <si>
+    <t>IMG20</t>
+  </si>
+  <si>
+    <t>IMG09</t>
+  </si>
+  <si>
+    <t>IMG10</t>
+  </si>
+  <si>
+    <t>IMG11</t>
+  </si>
+  <si>
+    <t>IMG12</t>
+  </si>
+  <si>
+    <t>IMG13</t>
+  </si>
+  <si>
+    <t>IMG14</t>
+  </si>
+  <si>
+    <t>IMG15</t>
+  </si>
+  <si>
+    <t>IMG16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">División exacta </t>
+  </si>
+  <si>
+    <t>350 136</t>
+  </si>
+  <si>
+    <t>Divisor</t>
+  </si>
+  <si>
+    <t>Cociente</t>
+  </si>
+  <si>
+    <t>División inexacta</t>
+  </si>
+  <si>
+    <t>Ecuaciones aditivas</t>
+  </si>
+  <si>
+    <t>Ecuaciones multiplicativas</t>
+  </si>
+  <si>
+    <t>IMG17</t>
+  </si>
+  <si>
+    <t>IMG18</t>
   </si>
 </sst>
 </file>
@@ -1292,7 +1346,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="110">
+  <cellXfs count="111">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1585,6 +1639,9 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="51">
@@ -1810,13 +1867,13 @@
       <xdr:col>10</xdr:col>
       <xdr:colOff>103187</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>55562</xdr:rowOff>
+      <xdr:rowOff>63500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>2222501</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>960437</xdr:rowOff>
+      <xdr:rowOff>968375</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1830,7 +1887,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="17430750" y="4238625"/>
+          <a:off x="17295812" y="4246563"/>
           <a:ext cx="2119314" cy="904875"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1894,57 +1951,14 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>103187</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>7937</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>1904999</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>881062</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="19" name="Imagen 18"/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
-        <a:srcRect l="41442" t="37228" r="15078" b="33968"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="17430750" y="6357937"/>
-          <a:ext cx="1801812" cy="873125"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{53640926-AAD7-44D8-BBD7-CCE9431645EC}">
-            <a14:shadowObscured xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main"/>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>10</xdr:col>
       <xdr:colOff>134937</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>71438</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>2159000</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>428626</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1953,7 +1967,7 @@
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -1988,13 +2002,13 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>63500</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>2182812</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>428625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2003,7 +2017,7 @@
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -2030,6 +2044,482 @@
             <a14:shadowObscured xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main"/>
           </a:ext>
         </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>277813</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>87317</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>2254250</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>1230312</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17470438" y="7008817"/>
+          <a:ext cx="1976437" cy="1142995"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>134938</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>79375</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>2293938</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>1222374</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17327563" y="8374063"/>
+          <a:ext cx="2159000" cy="1142999"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>277812</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>55562</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>2087336</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>912705</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Imagen 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17470437" y="9628187"/>
+          <a:ext cx="1809524" cy="857143"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>87311</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>47623</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>2365374</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>1654968</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Imagen 12"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17256124" y="11287123"/>
+          <a:ext cx="2278063" cy="1607345"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>105832</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>116417</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>2391833</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>1386417</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Imagen 14"/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17303749" y="13091584"/>
+          <a:ext cx="2286001" cy="1270000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>116416</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>116416</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>2455333</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>1047750</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Imagen 15"/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17314333" y="14541499"/>
+          <a:ext cx="2338917" cy="931334"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>137583</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>52916</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>2402417</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>986366</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="18" name="Imagen 17"/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17335500" y="15705666"/>
+          <a:ext cx="2264834" cy="933450"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>52916</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>63499</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>2476500</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>1026582</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="20" name="Imagen 19"/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17250833" y="16785166"/>
+          <a:ext cx="2423584" cy="963083"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>63501</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>116416</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>2423583</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>973666</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="22" name="Imagen 21"/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17261418" y="18033999"/>
+          <a:ext cx="2360082" cy="857250"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>74082</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>105835</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>2444749</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>1005417</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="24" name="Imagen 23"/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17271999" y="19092335"/>
+          <a:ext cx="2370667" cy="899582"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>84666</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>2444746</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>1056216</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="25" name="Imagen 24"/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17293167" y="20214166"/>
+          <a:ext cx="2349496" cy="971550"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>74083</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>2423584</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>952500</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="26" name="Imagen 25"/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17293167" y="21336000"/>
+          <a:ext cx="2328334" cy="878417"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>105832</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>137583</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>2452157</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>1051983</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="27" name="Imagen 26"/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17303749" y="22468416"/>
+          <a:ext cx="2346325" cy="914400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -2750,11 +3240,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Hoja1"/>
-  <dimension ref="A1:P101"/>
+  <dimension ref="A1:P113"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="140" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="140" workbookViewId="0">
+      <pane ySplit="9" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -2768,8 +3258,8 @@
     <col min="7" max="7" width="20.5" style="2" customWidth="1"/>
     <col min="8" max="8" width="28.625" style="2" customWidth="1"/>
     <col min="9" max="9" width="20.5" style="2" customWidth="1"/>
-    <col min="10" max="10" width="34.875" style="17" customWidth="1"/>
-    <col min="11" max="11" width="29.625" style="17" customWidth="1"/>
+    <col min="10" max="10" width="33.125" style="17" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="33.125" style="17" customWidth="1"/>
     <col min="12" max="12" width="20.375" style="2" customWidth="1"/>
     <col min="13" max="13" width="14.5" style="2" customWidth="1"/>
     <col min="14" max="16384" width="10.875" style="2"/>
@@ -2911,7 +3401,7 @@
       <c r="O8" s="2"/>
       <c r="P8" s="2"/>
     </row>
-    <row r="9" spans="1:16" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" ht="69.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="28" t="s">
         <v>2</v>
       </c>
@@ -2954,7 +3444,7 @@
         <v>158</v>
       </c>
       <c r="C10" s="26" t="str">
-        <f t="shared" ref="C10:C67" si="0">IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
+        <f t="shared" ref="C10:C79" si="0">IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D10" s="14" t="s">
@@ -2964,7 +3454,7 @@
         <v>154</v>
       </c>
       <c r="F10" s="14" t="str">
-        <f t="shared" ref="F10:F67" si="1">IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),CONCATENATE($C$7,"_",$A10,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I10="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
+        <f t="shared" ref="F10:F79" si="1">IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),CONCATENATE($C$7,"_",$A10,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I10="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
         <v>MA_06_03_CO_IMG01_small</v>
       </c>
       <c r="G10" s="14" t="str">
@@ -2972,7 +3462,7 @@
         <v>526 x 370 px</v>
       </c>
       <c r="H10" s="14" t="str">
-        <f t="shared" ref="H10:H67" si="2">IF(AND(I10&lt;&gt;"",I10&lt;&gt;0),IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),CONCATENATE($C$7,"_",$A10,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+        <f t="shared" ref="H10:H79" si="2">IF(AND(I10&lt;&gt;"",I10&lt;&gt;0),IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),CONCATENATE($C$7,"_",$A10,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
         <v>MA_06_03_CO_IMG01_zoom</v>
       </c>
       <c r="I10" s="14" t="str">
@@ -3097,7 +3587,7 @@
         <v>157</v>
       </c>
       <c r="K13" s="20" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="14" spans="1:16" s="12" customFormat="1" ht="128.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3137,21 +3627,21 @@
         <v>162</v>
       </c>
       <c r="K14" s="20" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" s="12" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" s="12" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
         <v>152</v>
       </c>
-      <c r="B15" s="73" t="s">
+      <c r="B15" s="14" t="s">
         <v>158</v>
       </c>
       <c r="C15" s="26" t="str">
         <f t="shared" si="0"/>
         <v>Cuaderno de Estudio</v>
       </c>
-      <c r="D15" s="76" t="s">
+      <c r="D15" s="14" t="s">
         <v>156</v>
       </c>
       <c r="E15" s="14" t="s">
@@ -3173,16 +3663,23 @@
         <f>IF(OR(B15&lt;&gt;"",J15&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J15" s="76" t="s">
-        <v>163</v>
-      </c>
-      <c r="K15" s="74" t="s">
+      <c r="J15" s="14" t="s">
+        <v>180</v>
+      </c>
+      <c r="K15" s="110"/>
+      <c r="L15" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="M15" s="12">
+        <v>24</v>
+      </c>
+      <c r="N15" s="12" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" s="12" customFormat="1" ht="100.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="13" t="s">
         <v>164</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" s="12" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="13" t="s">
-        <v>165</v>
       </c>
       <c r="B16" s="73" t="s">
         <v>158</v>
@@ -3214,13 +3711,22 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J16" s="76" t="s">
+        <v>184</v>
+      </c>
+      <c r="K16" s="74"/>
+      <c r="L16" s="12">
+        <v>110</v>
+      </c>
+      <c r="M16" s="12">
+        <v>14589</v>
+      </c>
+      <c r="N16" s="12" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" s="12" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="13" t="s">
         <v>166</v>
-      </c>
-      <c r="K16" s="19"/>
-    </row>
-    <row r="17" spans="1:11" s="12" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="13" t="s">
-        <v>167</v>
       </c>
       <c r="B17" s="73" t="s">
         <v>158</v>
@@ -3252,385 +3758,472 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J17" s="76" t="s">
-        <v>168</v>
-      </c>
-      <c r="K17" s="15"/>
-    </row>
-    <row r="18" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="13" t="str">
-        <f t="shared" ref="A18:A76" si="3">IF(OR(B18&lt;&gt;"",J18&lt;&gt;""),CONCATENATE(LEFT(A17,3),IF(MID(A17,4,2)+1&lt;10,CONCATENATE("0",MID(A17,4,2)+1),MID(A17,4,2)+1)),"")</f>
-        <v/>
-      </c>
-      <c r="B18" s="13"/>
+        <v>184</v>
+      </c>
+      <c r="K17" s="74"/>
+      <c r="L17" s="12">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" s="12" customFormat="1" ht="136.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="13" t="s">
+        <v>172</v>
+      </c>
+      <c r="B18" s="73" t="s">
+        <v>158</v>
+      </c>
       <c r="C18" s="26" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
+        <f>IF(OR(B18&lt;&gt;"",J18&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
+        <v>Cuaderno de Estudio</v>
+      </c>
+      <c r="D18" s="26" t="str">
+        <f>IF(OR(C18&lt;&gt;"",K18&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
+        <v>Cuaderno de Estudio</v>
+      </c>
+      <c r="E18" s="14" t="s">
+        <v>154</v>
+      </c>
       <c r="F18" s="14" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>MA_06_03_CO_IMG09_small</v>
       </c>
       <c r="G18" s="14" t="str">
         <f>IF(F18&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
-        <v/>
+        <v>526 x 370 px</v>
       </c>
       <c r="H18" s="14" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>MA_06_03_CO_IMG09_zoom</v>
       </c>
       <c r="I18" s="14" t="str">
         <f>IF(OR(B18&lt;&gt;"",J18&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v/>
-      </c>
-      <c r="J18" s="14"/>
-      <c r="K18" s="19"/>
-    </row>
-    <row r="19" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="13" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="B19" s="13"/>
+        <v>800 x 600 px</v>
+      </c>
+      <c r="J18" s="76" t="s">
+        <v>163</v>
+      </c>
+      <c r="K18" s="74"/>
+      <c r="L18" s="12">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" s="12" customFormat="1" ht="114" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="B19" s="73" t="s">
+        <v>158</v>
+      </c>
       <c r="C19" s="26" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
+        <v>Cuaderno de Estudio</v>
+      </c>
+      <c r="D19" s="76" t="s">
+        <v>156</v>
+      </c>
+      <c r="E19" s="14" t="s">
+        <v>154</v>
+      </c>
       <c r="F19" s="14" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>MA_06_03_CO_IMG10_small</v>
       </c>
       <c r="G19" s="14" t="str">
         <f>IF(F19&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
-        <v/>
+        <v>526 x 370 px</v>
       </c>
       <c r="H19" s="14" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>MA_06_03_CO_IMG10_zoom</v>
       </c>
       <c r="I19" s="14" t="str">
         <f>IF(OR(B19&lt;&gt;"",J19&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v/>
-      </c>
-      <c r="J19" s="14"/>
-      <c r="K19" s="19"/>
-    </row>
-    <row r="20" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="13" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="B20" s="13"/>
+        <v>800 x 600 px</v>
+      </c>
+      <c r="J19" s="76" t="s">
+        <v>185</v>
+      </c>
+      <c r="K19" s="74"/>
+    </row>
+    <row r="20" spans="1:12" s="12" customFormat="1" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="13" t="s">
+        <v>174</v>
+      </c>
+      <c r="B20" s="73" t="s">
+        <v>158</v>
+      </c>
       <c r="C20" s="26" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
+        <v>Cuaderno de Estudio</v>
+      </c>
+      <c r="D20" s="76" t="s">
+        <v>156</v>
+      </c>
+      <c r="E20" s="14" t="s">
+        <v>154</v>
+      </c>
       <c r="F20" s="14" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>MA_06_03_CO_IMG11_small</v>
       </c>
       <c r="G20" s="14" t="str">
         <f>IF(F20&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
-        <v/>
+        <v>526 x 370 px</v>
       </c>
       <c r="H20" s="14" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>MA_06_03_CO_IMG11_zoom</v>
       </c>
       <c r="I20" s="14" t="str">
         <f>IF(OR(B20&lt;&gt;"",J20&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v/>
-      </c>
-      <c r="J20" s="19"/>
-      <c r="K20" s="19"/>
-    </row>
-    <row r="21" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="13" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="B21" s="13"/>
+        <v>800 x 600 px</v>
+      </c>
+      <c r="J20" s="76" t="s">
+        <v>185</v>
+      </c>
+      <c r="K20" s="74"/>
+    </row>
+    <row r="21" spans="1:12" s="12" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="13" t="s">
+        <v>175</v>
+      </c>
+      <c r="B21" s="73" t="s">
+        <v>158</v>
+      </c>
       <c r="C21" s="26" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
+        <v>Cuaderno de Estudio</v>
+      </c>
+      <c r="D21" s="76" t="s">
+        <v>156</v>
+      </c>
+      <c r="E21" s="14" t="s">
+        <v>154</v>
+      </c>
       <c r="F21" s="14" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>MA_06_03_CO_IMG12_small</v>
       </c>
       <c r="G21" s="14" t="str">
         <f>IF(F21&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
-        <v/>
+        <v>526 x 370 px</v>
       </c>
       <c r="H21" s="14" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>MA_06_03_CO_IMG12_zoom</v>
       </c>
       <c r="I21" s="14" t="str">
         <f>IF(OR(B21&lt;&gt;"",J21&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v/>
-      </c>
-      <c r="J21" s="19"/>
-      <c r="K21" s="19"/>
-    </row>
-    <row r="22" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="13" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="B22" s="13"/>
+        <v>800 x 600 px</v>
+      </c>
+      <c r="J21" s="76" t="s">
+        <v>185</v>
+      </c>
+      <c r="K21" s="74"/>
+    </row>
+    <row r="22" spans="1:12" s="12" customFormat="1" ht="93.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="13" t="s">
+        <v>176</v>
+      </c>
+      <c r="B22" s="73" t="s">
+        <v>158</v>
+      </c>
       <c r="C22" s="26" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
+        <v>Cuaderno de Estudio</v>
+      </c>
+      <c r="D22" s="76" t="s">
+        <v>156</v>
+      </c>
+      <c r="E22" s="14" t="s">
+        <v>154</v>
+      </c>
       <c r="F22" s="14" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>MA_06_03_CO_IMG13_small</v>
       </c>
       <c r="G22" s="14" t="str">
         <f>IF(F22&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
-        <v/>
+        <v>526 x 370 px</v>
       </c>
       <c r="H22" s="14" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>MA_06_03_CO_IMG13_zoom</v>
       </c>
       <c r="I22" s="14" t="str">
         <f>IF(OR(B22&lt;&gt;"",J22&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v/>
-      </c>
-      <c r="J22" s="19"/>
-      <c r="K22" s="19"/>
-    </row>
-    <row r="23" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="13" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="B23" s="13"/>
+        <v>800 x 600 px</v>
+      </c>
+      <c r="J22" s="76" t="s">
+        <v>185</v>
+      </c>
+      <c r="K22" s="74"/>
+    </row>
+    <row r="23" spans="1:12" s="12" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="13" t="s">
+        <v>177</v>
+      </c>
+      <c r="B23" s="73" t="s">
+        <v>158</v>
+      </c>
       <c r="C23" s="26" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="D23" s="14"/>
-      <c r="E23" s="14"/>
+        <v>Cuaderno de Estudio</v>
+      </c>
+      <c r="D23" s="76" t="s">
+        <v>156</v>
+      </c>
+      <c r="E23" s="14" t="s">
+        <v>154</v>
+      </c>
       <c r="F23" s="14" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>MA_06_03_CO_IMG14_small</v>
       </c>
       <c r="G23" s="14" t="str">
         <f>IF(F23&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
-        <v/>
+        <v>526 x 370 px</v>
       </c>
       <c r="H23" s="14" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>MA_06_03_CO_IMG14_zoom</v>
       </c>
       <c r="I23" s="14" t="str">
         <f>IF(OR(B23&lt;&gt;"",J23&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v/>
-      </c>
-      <c r="J23" s="19"/>
-      <c r="K23" s="19"/>
-    </row>
-    <row r="24" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="13" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="B24" s="13"/>
+        <v>800 x 600 px</v>
+      </c>
+      <c r="J23" s="76" t="s">
+        <v>185</v>
+      </c>
+      <c r="K23" s="74"/>
+    </row>
+    <row r="24" spans="1:12" s="12" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="13" t="s">
+        <v>178</v>
+      </c>
+      <c r="B24" s="73" t="s">
+        <v>158</v>
+      </c>
       <c r="C24" s="26" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="D24" s="14"/>
-      <c r="E24" s="14"/>
+        <v>Cuaderno de Estudio</v>
+      </c>
+      <c r="D24" s="76" t="s">
+        <v>156</v>
+      </c>
+      <c r="E24" s="14" t="s">
+        <v>154</v>
+      </c>
       <c r="F24" s="14" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>MA_06_03_CO_IMG15_small</v>
       </c>
       <c r="G24" s="14" t="str">
         <f>IF(F24&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
-        <v/>
+        <v>526 x 370 px</v>
       </c>
       <c r="H24" s="14" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>MA_06_03_CO_IMG15_zoom</v>
       </c>
       <c r="I24" s="14" t="str">
         <f>IF(OR(B24&lt;&gt;"",J24&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v/>
-      </c>
-      <c r="J24" s="19"/>
-      <c r="K24" s="19"/>
-    </row>
-    <row r="25" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="13" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="B25" s="13"/>
+        <v>800 x 600 px</v>
+      </c>
+      <c r="J24" s="76" t="s">
+        <v>186</v>
+      </c>
+      <c r="K24" s="74"/>
+    </row>
+    <row r="25" spans="1:12" s="12" customFormat="1" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="13" t="s">
+        <v>179</v>
+      </c>
+      <c r="B25" s="73" t="s">
+        <v>158</v>
+      </c>
       <c r="C25" s="26" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="D25" s="14"/>
-      <c r="E25" s="14"/>
+        <v>Cuaderno de Estudio</v>
+      </c>
+      <c r="D25" s="76" t="s">
+        <v>156</v>
+      </c>
+      <c r="E25" s="14" t="s">
+        <v>154</v>
+      </c>
       <c r="F25" s="14" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>MA_06_03_CO_IMG16_small</v>
       </c>
       <c r="G25" s="14" t="str">
         <f>IF(F25&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
-        <v/>
+        <v>526 x 370 px</v>
       </c>
       <c r="H25" s="14" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>MA_06_03_CO_IMG16_zoom</v>
       </c>
       <c r="I25" s="14" t="str">
         <f>IF(OR(B25&lt;&gt;"",J25&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v/>
-      </c>
-      <c r="J25" s="19"/>
-      <c r="K25" s="19"/>
-    </row>
-    <row r="26" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="13" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="B26" s="13"/>
+        <v>800 x 600 px</v>
+      </c>
+      <c r="J25" s="76" t="s">
+        <v>186</v>
+      </c>
+      <c r="K25" s="74"/>
+    </row>
+    <row r="26" spans="1:12" s="12" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="13" t="s">
+        <v>187</v>
+      </c>
+      <c r="B26" s="73" t="s">
+        <v>158</v>
+      </c>
       <c r="C26" s="26" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="D26" s="14"/>
-      <c r="E26" s="14"/>
+        <v>Cuaderno de Estudio</v>
+      </c>
+      <c r="D26" s="76" t="s">
+        <v>156</v>
+      </c>
+      <c r="E26" s="14" t="s">
+        <v>154</v>
+      </c>
       <c r="F26" s="14" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>MA_06_03_CO_IMG17_small</v>
       </c>
       <c r="G26" s="14" t="str">
         <f>IF(F26&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
-        <v/>
-      </c>
-      <c r="H26" s="14" t="str">
-        <f t="shared" si="2"/>
-        <v/>
+        <v>526 x 370 px</v>
       </c>
       <c r="I26" s="14" t="str">
         <f>IF(OR(B26&lt;&gt;"",J26&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v/>
-      </c>
-      <c r="J26" s="19"/>
-      <c r="K26" s="19"/>
-    </row>
-    <row r="27" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="13" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="B27" s="13"/>
+        <v>800 x 600 px</v>
+      </c>
+      <c r="J26" s="76" t="s">
+        <v>186</v>
+      </c>
+      <c r="K26" s="74"/>
+    </row>
+    <row r="27" spans="1:12" s="12" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="13" t="s">
+        <v>188</v>
+      </c>
+      <c r="B27" s="73" t="s">
+        <v>158</v>
+      </c>
       <c r="C27" s="26" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14"/>
+        <v>Cuaderno de Estudio</v>
+      </c>
+      <c r="D27" s="76" t="s">
+        <v>156</v>
+      </c>
+      <c r="E27" s="14" t="s">
+        <v>154</v>
+      </c>
       <c r="F27" s="14" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>MA_06_03_CO_IMG18_small</v>
       </c>
       <c r="G27" s="14" t="str">
         <f>IF(F27&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
-        <v/>
+        <v>526 x 370 px</v>
       </c>
       <c r="H27" s="14" t="str">
-        <f t="shared" si="2"/>
-        <v/>
+        <f>IF(AND(I26&lt;&gt;"",I26&lt;&gt;0),IF(OR(B26&lt;&gt;"",J26&lt;&gt;""),CONCATENATE($C$7,"_",$A26,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+        <v>MA_06_03_CO_IMG17_zoom</v>
       </c>
       <c r="I27" s="14" t="str">
         <f>IF(OR(B27&lt;&gt;"",J27&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v/>
-      </c>
-      <c r="J27" s="19"/>
-      <c r="K27" s="19"/>
-    </row>
-    <row r="28" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="13" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="B28" s="13"/>
+        <v>800 x 600 px</v>
+      </c>
+      <c r="J27" s="76" t="s">
+        <v>186</v>
+      </c>
+      <c r="K27" s="74"/>
+    </row>
+    <row r="28" spans="1:12" s="12" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="13" t="s">
+        <v>170</v>
+      </c>
+      <c r="B28" s="73" t="s">
+        <v>158</v>
+      </c>
       <c r="C28" s="26" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="D28" s="14"/>
-      <c r="E28" s="14"/>
+        <v>Cuaderno de Estudio</v>
+      </c>
+      <c r="D28" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="E28" s="14" t="s">
+        <v>154</v>
+      </c>
       <c r="F28" s="14" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>MA_06_03_CO_IMG19_small</v>
       </c>
       <c r="G28" s="14" t="str">
         <f>IF(F28&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
-        <v/>
+        <v>526 x 370 px</v>
       </c>
       <c r="H28" s="14" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>MA_06_03_CO_IMG19_zoom</v>
       </c>
       <c r="I28" s="14" t="str">
         <f>IF(OR(B28&lt;&gt;"",J28&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v/>
-      </c>
-      <c r="J28" s="14"/>
-      <c r="K28" s="15"/>
-    </row>
-    <row r="29" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="13" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="B29" s="13"/>
+        <v>800 x 600 px</v>
+      </c>
+      <c r="J28" s="76" t="s">
+        <v>165</v>
+      </c>
+      <c r="K28" s="19"/>
+    </row>
+    <row r="29" spans="1:12" s="12" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="13" t="s">
+        <v>171</v>
+      </c>
+      <c r="B29" s="73" t="s">
+        <v>158</v>
+      </c>
       <c r="C29" s="26" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="D29" s="14"/>
-      <c r="E29" s="14"/>
+        <v>Cuaderno de Estudio</v>
+      </c>
+      <c r="D29" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="E29" s="14" t="s">
+        <v>154</v>
+      </c>
       <c r="F29" s="14" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>MA_06_03_CO_IMG20_small</v>
       </c>
       <c r="G29" s="14" t="str">
         <f>IF(F29&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
-        <v/>
+        <v>526 x 370 px</v>
       </c>
       <c r="H29" s="14" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>MA_06_03_CO_IMG20_zoom</v>
       </c>
       <c r="I29" s="14" t="str">
         <f>IF(OR(B29&lt;&gt;"",J29&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v/>
-      </c>
-      <c r="J29" s="14"/>
+        <v>800 x 600 px</v>
+      </c>
+      <c r="J29" s="76" t="s">
+        <v>167</v>
+      </c>
       <c r="K29" s="15"/>
     </row>
-    <row r="30" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="13" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="A30:A88" si="3">IF(OR(B30&lt;&gt;"",J30&lt;&gt;""),CONCATENATE(LEFT(A29,3),IF(MID(A29,4,2)+1&lt;10,CONCATENATE("0",MID(A29,4,2)+1),MID(A29,4,2)+1)),"")</f>
         <v/>
       </c>
       <c r="B30" s="13"/>
@@ -3656,10 +4249,10 @@
         <f>IF(OR(B30&lt;&gt;"",J30&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
-      <c r="J30" s="21"/>
-      <c r="K30" s="15"/>
-    </row>
-    <row r="31" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J30" s="14"/>
+      <c r="K30" s="19"/>
+    </row>
+    <row r="31" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -3687,10 +4280,10 @@
         <f>IF(OR(B31&lt;&gt;"",J31&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
-      <c r="J31" s="22"/>
-      <c r="K31" s="15"/>
-    </row>
-    <row r="32" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J31" s="14"/>
+      <c r="K31" s="19"/>
+    </row>
+    <row r="32" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -3718,8 +4311,8 @@
         <f>IF(OR(B32&lt;&gt;"",J32&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
-      <c r="J32" s="14"/>
-      <c r="K32" s="15"/>
+      <c r="J32" s="19"/>
+      <c r="K32" s="19"/>
     </row>
     <row r="33" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="str">
@@ -3749,8 +4342,8 @@
         <f>IF(OR(B33&lt;&gt;"",J33&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
-      <c r="J33" s="14"/>
-      <c r="K33" s="15"/>
+      <c r="J33" s="19"/>
+      <c r="K33" s="19"/>
     </row>
     <row r="34" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="13" t="str">
@@ -3780,8 +4373,8 @@
         <f>IF(OR(B34&lt;&gt;"",J34&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
-      <c r="J34" s="14"/>
-      <c r="K34" s="15"/>
+      <c r="J34" s="19"/>
+      <c r="K34" s="19"/>
     </row>
     <row r="35" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="13" t="str">
@@ -3811,8 +4404,8 @@
         <f>IF(OR(B35&lt;&gt;"",J35&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
-      <c r="J35" s="14"/>
-      <c r="K35" s="15"/>
+      <c r="J35" s="19"/>
+      <c r="K35" s="19"/>
     </row>
     <row r="36" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="13" t="str">
@@ -3842,8 +4435,8 @@
         <f>IF(OR(B36&lt;&gt;"",J36&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
-      <c r="J36" s="14"/>
-      <c r="K36" s="15"/>
+      <c r="J36" s="19"/>
+      <c r="K36" s="19"/>
     </row>
     <row r="37" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="13" t="str">
@@ -3873,8 +4466,8 @@
         <f>IF(OR(B37&lt;&gt;"",J37&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
-      <c r="J37" s="14"/>
-      <c r="K37" s="15"/>
+      <c r="J37" s="19"/>
+      <c r="K37" s="19"/>
     </row>
     <row r="38" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="13" t="str">
@@ -3904,8 +4497,8 @@
         <f>IF(OR(B38&lt;&gt;"",J38&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
-      <c r="J38" s="14"/>
-      <c r="K38" s="15"/>
+      <c r="J38" s="19"/>
+      <c r="K38" s="19"/>
     </row>
     <row r="39" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="13" t="str">
@@ -3935,8 +4528,8 @@
         <f>IF(OR(B39&lt;&gt;"",J39&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
-      <c r="J39" s="14"/>
-      <c r="K39" s="15"/>
+      <c r="J39" s="19"/>
+      <c r="K39" s="19"/>
     </row>
     <row r="40" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="13" t="str">
@@ -4028,7 +4621,7 @@
         <f>IF(OR(B42&lt;&gt;"",J42&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
-      <c r="J42" s="14"/>
+      <c r="J42" s="21"/>
       <c r="K42" s="15"/>
     </row>
     <row r="43" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -4059,7 +4652,7 @@
         <f>IF(OR(B43&lt;&gt;"",J43&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
-      <c r="J43" s="14"/>
+      <c r="J43" s="22"/>
       <c r="K43" s="15"/>
     </row>
     <row r="44" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -4813,13 +5406,13 @@
       </c>
       <c r="B68" s="13"/>
       <c r="C68" s="26" t="str">
-        <f t="shared" ref="C68:C101" si="4">IF(OR(B68&lt;&gt;"",J68&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="D68" s="14"/>
       <c r="E68" s="14"/>
       <c r="F68" s="14" t="str">
-        <f t="shared" ref="F68:F101" si="5">IF(OR(B68&lt;&gt;"",J68&lt;&gt;""),CONCATENATE($C$7,"_",$A68,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I68="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="G68" s="14" t="str">
@@ -4827,7 +5420,7 @@
         <v/>
       </c>
       <c r="H68" s="14" t="str">
-        <f t="shared" ref="H68:H101" si="6">IF(AND(I68&lt;&gt;"",I68&lt;&gt;0),IF(OR(B68&lt;&gt;"",J68&lt;&gt;""),CONCATENATE($C$7,"_",$A68,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="I68" s="14" t="str">
@@ -4844,13 +5437,13 @@
       </c>
       <c r="B69" s="13"/>
       <c r="C69" s="26" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="D69" s="14"/>
       <c r="E69" s="14"/>
       <c r="F69" s="14" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="G69" s="14" t="str">
@@ -4858,7 +5451,7 @@
         <v/>
       </c>
       <c r="H69" s="14" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="I69" s="14" t="str">
@@ -4875,13 +5468,13 @@
       </c>
       <c r="B70" s="13"/>
       <c r="C70" s="26" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="D70" s="14"/>
       <c r="E70" s="14"/>
       <c r="F70" s="14" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="G70" s="14" t="str">
@@ -4889,7 +5482,7 @@
         <v/>
       </c>
       <c r="H70" s="14" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="I70" s="14" t="str">
@@ -4906,13 +5499,13 @@
       </c>
       <c r="B71" s="13"/>
       <c r="C71" s="26" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="D71" s="14"/>
       <c r="E71" s="14"/>
       <c r="F71" s="14" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="G71" s="14" t="str">
@@ -4920,7 +5513,7 @@
         <v/>
       </c>
       <c r="H71" s="14" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="I71" s="14" t="str">
@@ -4937,13 +5530,13 @@
       </c>
       <c r="B72" s="13"/>
       <c r="C72" s="26" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="D72" s="14"/>
       <c r="E72" s="14"/>
       <c r="F72" s="14" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="G72" s="14" t="str">
@@ -4951,7 +5544,7 @@
         <v/>
       </c>
       <c r="H72" s="14" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="I72" s="14" t="str">
@@ -4968,13 +5561,13 @@
       </c>
       <c r="B73" s="13"/>
       <c r="C73" s="26" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="D73" s="14"/>
       <c r="E73" s="14"/>
       <c r="F73" s="14" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="G73" s="14" t="str">
@@ -4982,7 +5575,7 @@
         <v/>
       </c>
       <c r="H73" s="14" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="I73" s="14" t="str">
@@ -4999,13 +5592,13 @@
       </c>
       <c r="B74" s="13"/>
       <c r="C74" s="26" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="D74" s="14"/>
       <c r="E74" s="14"/>
       <c r="F74" s="14" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="G74" s="14" t="str">
@@ -5013,7 +5606,7 @@
         <v/>
       </c>
       <c r="H74" s="14" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="I74" s="14" t="str">
@@ -5030,13 +5623,13 @@
       </c>
       <c r="B75" s="13"/>
       <c r="C75" s="26" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="D75" s="14"/>
       <c r="E75" s="14"/>
       <c r="F75" s="14" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="G75" s="14" t="str">
@@ -5044,7 +5637,7 @@
         <v/>
       </c>
       <c r="H75" s="14" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="I75" s="14" t="str">
@@ -5061,13 +5654,13 @@
       </c>
       <c r="B76" s="13"/>
       <c r="C76" s="26" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="D76" s="14"/>
       <c r="E76" s="14"/>
       <c r="F76" s="14" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="G76" s="14" t="str">
@@ -5075,7 +5668,7 @@
         <v/>
       </c>
       <c r="H76" s="14" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="I76" s="14" t="str">
@@ -5087,18 +5680,18 @@
     </row>
     <row r="77" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="13" t="str">
-        <f t="shared" ref="A77:A101" si="7">IF(OR(B77&lt;&gt;"",J77&lt;&gt;""),CONCATENATE(LEFT(A76,3),IF(MID(A76,4,2)+1&lt;10,CONCATENATE("0",MID(A76,4,2)+1),MID(A76,4,2)+1)),"")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="B77" s="13"/>
       <c r="C77" s="26" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="D77" s="14"/>
       <c r="E77" s="14"/>
       <c r="F77" s="14" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="G77" s="14" t="str">
@@ -5106,7 +5699,7 @@
         <v/>
       </c>
       <c r="H77" s="14" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="I77" s="14" t="str">
@@ -5118,18 +5711,18 @@
     </row>
     <row r="78" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="13" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="B78" s="13"/>
       <c r="C78" s="26" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="D78" s="14"/>
       <c r="E78" s="14"/>
       <c r="F78" s="14" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="G78" s="14" t="str">
@@ -5137,7 +5730,7 @@
         <v/>
       </c>
       <c r="H78" s="14" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="I78" s="14" t="str">
@@ -5149,18 +5742,18 @@
     </row>
     <row r="79" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="13" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="B79" s="13"/>
       <c r="C79" s="26" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="D79" s="14"/>
       <c r="E79" s="14"/>
       <c r="F79" s="14" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="G79" s="14" t="str">
@@ -5168,7 +5761,7 @@
         <v/>
       </c>
       <c r="H79" s="14" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="I79" s="14" t="str">
@@ -5180,18 +5773,18 @@
     </row>
     <row r="80" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="13" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="B80" s="13"/>
       <c r="C80" s="26" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="C80:C113" si="4">IF(OR(B80&lt;&gt;"",J80&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
         <v/>
       </c>
       <c r="D80" s="14"/>
       <c r="E80" s="14"/>
       <c r="F80" s="14" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="F80:F113" si="5">IF(OR(B80&lt;&gt;"",J80&lt;&gt;""),CONCATENATE($C$7,"_",$A80,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I80="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
         <v/>
       </c>
       <c r="G80" s="14" t="str">
@@ -5199,7 +5792,7 @@
         <v/>
       </c>
       <c r="H80" s="14" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="H80:H113" si="6">IF(AND(I80&lt;&gt;"",I80&lt;&gt;0),IF(OR(B80&lt;&gt;"",J80&lt;&gt;""),CONCATENATE($C$7,"_",$A80,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
         <v/>
       </c>
       <c r="I80" s="14" t="str">
@@ -5211,7 +5804,7 @@
     </row>
     <row r="81" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="13" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="B81" s="13"/>
@@ -5242,7 +5835,7 @@
     </row>
     <row r="82" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="13" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="B82" s="13"/>
@@ -5273,7 +5866,7 @@
     </row>
     <row r="83" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="13" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="B83" s="13"/>
@@ -5304,7 +5897,7 @@
     </row>
     <row r="84" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="13" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="B84" s="13"/>
@@ -5335,7 +5928,7 @@
     </row>
     <row r="85" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="13" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="B85" s="13"/>
@@ -5366,7 +5959,7 @@
     </row>
     <row r="86" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" s="13" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="B86" s="13"/>
@@ -5397,7 +5990,7 @@
     </row>
     <row r="87" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="13" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="B87" s="13"/>
@@ -5428,7 +6021,7 @@
     </row>
     <row r="88" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A88" s="13" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="B88" s="13"/>
@@ -5459,7 +6052,7 @@
     </row>
     <row r="89" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" s="13" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" ref="A89:A113" si="7">IF(OR(B89&lt;&gt;"",J89&lt;&gt;""),CONCATENATE(LEFT(A88,3),IF(MID(A88,4,2)+1&lt;10,CONCATENATE("0",MID(A88,4,2)+1),MID(A88,4,2)+1)),"")</f>
         <v/>
       </c>
       <c r="B89" s="13"/>
@@ -5859,6 +6452,378 @@
       </c>
       <c r="J101" s="14"/>
       <c r="K101" s="15"/>
+    </row>
+    <row r="102" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A102" s="13" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="B102" s="13"/>
+      <c r="C102" s="26" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="D102" s="14"/>
+      <c r="E102" s="14"/>
+      <c r="F102" s="14" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="G102" s="14" t="str">
+        <f>IF(F102&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
+        <v/>
+      </c>
+      <c r="H102" s="14" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="I102" s="14" t="str">
+        <f>IF(OR(B102&lt;&gt;"",J102&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <v/>
+      </c>
+      <c r="J102" s="14"/>
+      <c r="K102" s="15"/>
+    </row>
+    <row r="103" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A103" s="13" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="B103" s="13"/>
+      <c r="C103" s="26" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="D103" s="14"/>
+      <c r="E103" s="14"/>
+      <c r="F103" s="14" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="G103" s="14" t="str">
+        <f>IF(F103&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
+        <v/>
+      </c>
+      <c r="H103" s="14" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="I103" s="14" t="str">
+        <f>IF(OR(B103&lt;&gt;"",J103&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <v/>
+      </c>
+      <c r="J103" s="14"/>
+      <c r="K103" s="15"/>
+    </row>
+    <row r="104" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A104" s="13" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="B104" s="13"/>
+      <c r="C104" s="26" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="D104" s="14"/>
+      <c r="E104" s="14"/>
+      <c r="F104" s="14" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="G104" s="14" t="str">
+        <f>IF(F104&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
+        <v/>
+      </c>
+      <c r="H104" s="14" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="I104" s="14" t="str">
+        <f>IF(OR(B104&lt;&gt;"",J104&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <v/>
+      </c>
+      <c r="J104" s="14"/>
+      <c r="K104" s="15"/>
+    </row>
+    <row r="105" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A105" s="13" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="B105" s="13"/>
+      <c r="C105" s="26" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="D105" s="14"/>
+      <c r="E105" s="14"/>
+      <c r="F105" s="14" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="G105" s="14" t="str">
+        <f>IF(F105&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
+        <v/>
+      </c>
+      <c r="H105" s="14" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="I105" s="14" t="str">
+        <f>IF(OR(B105&lt;&gt;"",J105&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <v/>
+      </c>
+      <c r="J105" s="14"/>
+      <c r="K105" s="15"/>
+    </row>
+    <row r="106" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A106" s="13" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="B106" s="13"/>
+      <c r="C106" s="26" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="D106" s="14"/>
+      <c r="E106" s="14"/>
+      <c r="F106" s="14" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="G106" s="14" t="str">
+        <f>IF(F106&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
+        <v/>
+      </c>
+      <c r="H106" s="14" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="I106" s="14" t="str">
+        <f>IF(OR(B106&lt;&gt;"",J106&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <v/>
+      </c>
+      <c r="J106" s="14"/>
+      <c r="K106" s="15"/>
+    </row>
+    <row r="107" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A107" s="13" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="B107" s="13"/>
+      <c r="C107" s="26" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="D107" s="14"/>
+      <c r="E107" s="14"/>
+      <c r="F107" s="14" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="G107" s="14" t="str">
+        <f>IF(F107&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
+        <v/>
+      </c>
+      <c r="H107" s="14" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="I107" s="14" t="str">
+        <f>IF(OR(B107&lt;&gt;"",J107&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <v/>
+      </c>
+      <c r="J107" s="14"/>
+      <c r="K107" s="15"/>
+    </row>
+    <row r="108" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A108" s="13" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="B108" s="13"/>
+      <c r="C108" s="26" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="D108" s="14"/>
+      <c r="E108" s="14"/>
+      <c r="F108" s="14" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="G108" s="14" t="str">
+        <f>IF(F108&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
+        <v/>
+      </c>
+      <c r="H108" s="14" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="I108" s="14" t="str">
+        <f>IF(OR(B108&lt;&gt;"",J108&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <v/>
+      </c>
+      <c r="J108" s="14"/>
+      <c r="K108" s="15"/>
+    </row>
+    <row r="109" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A109" s="13" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="B109" s="13"/>
+      <c r="C109" s="26" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="D109" s="14"/>
+      <c r="E109" s="14"/>
+      <c r="F109" s="14" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="G109" s="14" t="str">
+        <f>IF(F109&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
+        <v/>
+      </c>
+      <c r="H109" s="14" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="I109" s="14" t="str">
+        <f>IF(OR(B109&lt;&gt;"",J109&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <v/>
+      </c>
+      <c r="J109" s="14"/>
+      <c r="K109" s="15"/>
+    </row>
+    <row r="110" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A110" s="13" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="B110" s="13"/>
+      <c r="C110" s="26" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="D110" s="14"/>
+      <c r="E110" s="14"/>
+      <c r="F110" s="14" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="G110" s="14" t="str">
+        <f>IF(F110&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
+        <v/>
+      </c>
+      <c r="H110" s="14" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="I110" s="14" t="str">
+        <f>IF(OR(B110&lt;&gt;"",J110&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <v/>
+      </c>
+      <c r="J110" s="14"/>
+      <c r="K110" s="15"/>
+    </row>
+    <row r="111" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A111" s="13" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="B111" s="13"/>
+      <c r="C111" s="26" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="D111" s="14"/>
+      <c r="E111" s="14"/>
+      <c r="F111" s="14" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="G111" s="14" t="str">
+        <f>IF(F111&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
+        <v/>
+      </c>
+      <c r="H111" s="14" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="I111" s="14" t="str">
+        <f>IF(OR(B111&lt;&gt;"",J111&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <v/>
+      </c>
+      <c r="J111" s="14"/>
+      <c r="K111" s="15"/>
+    </row>
+    <row r="112" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A112" s="13" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="B112" s="13"/>
+      <c r="C112" s="26" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="D112" s="14"/>
+      <c r="E112" s="14"/>
+      <c r="F112" s="14" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="G112" s="14" t="str">
+        <f>IF(F112&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
+        <v/>
+      </c>
+      <c r="H112" s="14" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="I112" s="14" t="str">
+        <f>IF(OR(B112&lt;&gt;"",J112&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <v/>
+      </c>
+      <c r="J112" s="14"/>
+      <c r="K112" s="15"/>
+    </row>
+    <row r="113" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A113" s="13" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="B113" s="13"/>
+      <c r="C113" s="26" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="D113" s="14"/>
+      <c r="E113" s="14"/>
+      <c r="F113" s="14" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="G113" s="14" t="str">
+        <f>IF(F113&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
+        <v/>
+      </c>
+      <c r="H113" s="14" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="I113" s="14" t="str">
+        <f>IF(OR(B113&lt;&gt;"",J113&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <v/>
+      </c>
+      <c r="J113" s="14"/>
+      <c r="K113" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -5900,10 +6865,10 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3">
       <formula1>"3,4,5,6,7,8,9,10,11"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E10:E101">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E10:E113">
       <formula1>"Vertical,Horizontal"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D10:D101">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D10:D17 D19:D113">
       <formula1>"Ilustración,Fotografía"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>